<commit_message>
Remove date cell from shimmingB file
</commit_message>
<xml_diff>
--- a/model-03/shimming_list/2023-04-24_delta_sabia_shimmingB_21periods.xlsx
+++ b/model-03/shimming_list/2023-04-24_delta_sabia_shimmingB_21periods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.francisco\data\2023-04_DeltaSabia-ShimB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.francisco\data\lnls-ima\id-sabia\model-03\shimming_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B883BE8F-2A6D-483F-976A-6194F9B8591B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37528D0C-1FE1-4B09-9158-5D1B5C51819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1505,7 +1505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1596,12 +1596,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1924,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,75 +1937,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
-        <v>45041</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>454</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>456</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>457</v>
+      <c r="A2" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="B2" s="15">
+        <v>-7.2917399999999997E-3</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1.3729089999999999E-2</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1.352456653</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="16">
+        <v>1</v>
+      </c>
+      <c r="I2" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="18">
+        <f t="shared" ref="K2:K33" si="0">I2+J2</f>
+        <v>0.25</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16">
+        <f>L2+K2</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B3" s="15">
-        <v>-7.2917399999999997E-3</v>
+        <v>-1.655734E-2</v>
       </c>
       <c r="C3" s="15">
-        <v>1.3729089999999999E-2</v>
+        <v>1.372335581</v>
       </c>
       <c r="D3" s="15">
-        <v>1.352456653</v>
+        <v>1.945979E-3</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>12</v>
@@ -2020,37 +2036,37 @@
         <v>372</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="18">
         <v>0.25</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="18">
-        <f t="shared" ref="K3:K34" si="0">I3+J3</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16">
-        <f>L3+K3</f>
+        <f t="shared" ref="M3:M66" si="1">L3+K3</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B4" s="15">
-        <v>-1.655734E-2</v>
+        <v>-2.3864139999999999E-3</v>
       </c>
       <c r="C4" s="15">
-        <v>1.372335581</v>
+        <v>1.6605050999999999E-2</v>
       </c>
       <c r="D4" s="15">
-        <v>1.945979E-3</v>
+        <v>-1.354623181</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>12</v>
@@ -2059,7 +2075,7 @@
         <v>372</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="16">
         <v>0</v>
@@ -2074,22 +2090,22 @@
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="16">
-        <f t="shared" ref="M4:M67" si="1">L4+K4</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B5" s="15">
-        <v>-2.3864139999999999E-3</v>
+        <v>9.7000130000000004E-3</v>
       </c>
       <c r="C5" s="15">
-        <v>1.6605050999999999E-2</v>
+        <v>9.8482229999999997E-3</v>
       </c>
       <c r="D5" s="15">
-        <v>-1.354623181</v>
+        <v>-1.3539807100000001</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>12</v>
@@ -2119,16 +2135,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>386</v>
+        <v>442</v>
       </c>
       <c r="B6" s="15">
-        <v>9.7000130000000004E-3</v>
+        <v>-1.6130582399759241E-2</v>
       </c>
       <c r="C6" s="15">
-        <v>9.8482229999999997E-3</v>
+        <v>-5.2596100935518326E-3</v>
       </c>
       <c r="D6" s="15">
-        <v>-1.3539807100000001</v>
+        <v>-1.3551642462419671</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>12</v>
@@ -2158,16 +2174,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B7" s="15">
-        <v>-1.6130582399759241E-2</v>
+        <v>3.1630300000000001E-5</v>
       </c>
       <c r="C7" s="15">
-        <v>-5.2596100935518326E-3</v>
+        <v>-1.3730064559999999</v>
       </c>
       <c r="D7" s="15">
-        <v>-1.3551642462419671</v>
+        <v>9.3682499999999996E-4</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>12</v>
@@ -2176,10 +2192,10 @@
         <v>372</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H7" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="18">
         <v>0.25</v>
@@ -2197,16 +2213,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B8" s="15">
-        <v>3.1630300000000001E-5</v>
+        <v>1.8529073E-2</v>
       </c>
       <c r="C8" s="15">
-        <v>-1.3730064559999999</v>
+        <v>-1.372854864</v>
       </c>
       <c r="D8" s="15">
-        <v>9.3682499999999996E-4</v>
+        <v>4.1514029999999997E-3</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>12</v>
@@ -2218,7 +2234,7 @@
         <v>38</v>
       </c>
       <c r="H8" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="18">
         <v>0.25</v>
@@ -2234,135 +2250,137 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1.8529073E-2</v>
-      </c>
-      <c r="C9" s="15">
-        <v>-1.372854864</v>
-      </c>
-      <c r="D9" s="15">
-        <v>4.1514029999999997E-3</v>
-      </c>
-      <c r="E9" s="16" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" s="29">
+        <v>-1.8492978E-2</v>
+      </c>
+      <c r="C9" s="29">
+        <v>-1.373798174</v>
+      </c>
+      <c r="D9" s="29">
+        <v>-3.2045400000000001E-3</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="30" t="s">
         <v>372</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="16">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="18">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>439</v>
-      </c>
-      <c r="B10" s="29">
-        <v>-1.8492978E-2</v>
-      </c>
-      <c r="C10" s="29">
-        <v>-1.373798174</v>
-      </c>
-      <c r="D10" s="29">
-        <v>-3.2045400000000001E-3</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="H9" s="28">
+        <v>1</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="31">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4.6740100000000001E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.5725062000000001E-2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.3639588920000001</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="G10" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="28">
-        <v>1</v>
-      </c>
-      <c r="I10" s="31">
-        <v>0.25</v>
-      </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="31">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28">
+      <c r="G10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="B11" s="5">
-        <v>4.6740100000000001E-3</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1.5725062000000001E-2</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.3639588920000001</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="A11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="15">
+        <v>-1.6537609999999999E-3</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.3711098070000001</v>
+      </c>
+      <c r="D11" s="15">
+        <v>5.1304499999999995E-4</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="7">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="18">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="L11" s="16">
+        <v>-4.9999999999999989E-2</v>
+      </c>
+      <c r="M11" s="16">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="15">
-        <v>-1.6537609999999999E-3</v>
+        <v>-9.0905729999999994E-3</v>
       </c>
       <c r="C12" s="15">
-        <v>1.3711098070000001</v>
+        <v>1.9718019999999999E-3</v>
       </c>
       <c r="D12" s="15">
-        <v>5.1304499999999995E-4</v>
+        <v>-1.3659446630000001</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>12</v>
@@ -2371,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="16">
         <v>0</v>
@@ -2384,26 +2402,24 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L12" s="16">
-        <v>-4.9999999999999989E-2</v>
-      </c>
+      <c r="L12" s="16"/>
       <c r="M12" s="16">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="15">
-        <v>-9.0905729999999994E-3</v>
+        <v>6.7145629999999998E-3</v>
       </c>
       <c r="C13" s="15">
-        <v>1.9718019999999999E-3</v>
+        <v>-1.3723693690000001</v>
       </c>
       <c r="D13" s="15">
-        <v>-1.3659446630000001</v>
+        <v>5.5409000000000003E-4</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>12</v>
@@ -2412,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H13" s="16">
         <v>0</v>
@@ -2425,24 +2441,26 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L13" s="16"/>
+      <c r="L13" s="16">
+        <v>4.9999999999999989E-2</v>
+      </c>
       <c r="M13" s="16">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B14" s="15">
-        <v>6.7145629999999998E-3</v>
+        <v>4.0084769999999999E-3</v>
       </c>
       <c r="C14" s="15">
-        <v>-1.3723693690000001</v>
+        <v>-7.2474900000000001E-4</v>
       </c>
       <c r="D14" s="15">
-        <v>5.5409000000000003E-4</v>
+        <v>1.3649628629999999</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>12</v>
@@ -2451,10 +2469,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="18">
         <v>0.25</v>
@@ -2464,65 +2482,65 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L14" s="16">
-        <v>4.9999999999999989E-2</v>
-      </c>
+      <c r="L14" s="16"/>
       <c r="M14" s="16">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="15">
-        <v>4.0084769999999999E-3</v>
-      </c>
-      <c r="C15" s="15">
-        <v>-7.2474900000000001E-4</v>
-      </c>
-      <c r="D15" s="15">
-        <v>1.3649628629999999</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="17">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="16">
-        <v>1</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="18">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+      <c r="A15" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-3.755736E-3</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1.368105991</v>
+      </c>
+      <c r="D15" s="12">
+        <v>4.8438000000000002E-4</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="13">
+        <v>2</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="14">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="L15" s="11">
+        <v>-4.9999999999999989E-2</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B16" s="12">
-        <v>-3.755736E-3</v>
+        <v>7.0072090000000004E-3</v>
       </c>
       <c r="C16" s="12">
-        <v>1.368105991</v>
+        <v>5.5113480000000001E-3</v>
       </c>
       <c r="D16" s="12">
-        <v>4.8438000000000002E-4</v>
+        <v>-1.3635150650000001</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>13</v>
@@ -2531,10 +2549,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="14">
         <v>0.25</v>
@@ -2544,26 +2562,24 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L16" s="11">
-        <v>-4.9999999999999989E-2</v>
-      </c>
+      <c r="L16" s="11"/>
       <c r="M16" s="11">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B17" s="12">
-        <v>7.0072090000000004E-3</v>
+        <v>1.0748914E-2</v>
       </c>
       <c r="C17" s="12">
-        <v>5.5113480000000001E-3</v>
+        <v>-1.367839134</v>
       </c>
       <c r="D17" s="12">
-        <v>-1.3635150650000001</v>
+        <v>-2.0662480000000001E-3</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>13</v>
@@ -2572,10 +2588,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H17" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="14">
         <v>0.25</v>
@@ -2585,24 +2601,26 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="11">
+        <v>4.9999999999999989E-2</v>
+      </c>
       <c r="M17" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B18" s="12">
-        <v>1.0748914E-2</v>
+        <v>-1.3809649E-2</v>
       </c>
       <c r="C18" s="12">
-        <v>-1.367839134</v>
+        <v>-5.6210050000000001E-3</v>
       </c>
       <c r="D18" s="12">
-        <v>-2.0662480000000001E-3</v>
+        <v>1.3652922519999999</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>13</v>
@@ -2611,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H18" s="11">
         <v>1</v>
@@ -2624,35 +2642,33 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L18" s="11">
-        <v>4.9999999999999989E-2</v>
-      </c>
+      <c r="L18" s="11"/>
       <c r="M18" s="11">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
       <c r="B19" s="12">
-        <v>-1.3809649E-2</v>
+        <v>-3.2737109999999999E-3</v>
       </c>
       <c r="C19" s="12">
-        <v>-5.6210050000000001E-3</v>
+        <v>1.3710564670000001</v>
       </c>
       <c r="D19" s="12">
-        <v>1.3652922519999999</v>
+        <v>8.4200499999999995E-5</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H19" s="11">
         <v>1</v>
@@ -2665,7 +2681,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L19" s="11"/>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
       <c r="M19" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2673,16 +2691,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="12">
-        <v>-3.2737109999999999E-3</v>
+        <v>7.9435400000000007E-3</v>
       </c>
       <c r="C20" s="12">
-        <v>1.3710564670000001</v>
+        <v>8.7541699999999997E-4</v>
       </c>
       <c r="D20" s="12">
-        <v>8.4200499999999995E-5</v>
+        <v>-1.3629746279999999</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>13</v>
@@ -2691,10 +2709,10 @@
         <v>3</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="14">
         <v>0.25</v>
@@ -2704,9 +2722,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L20" s="11">
-        <v>0</v>
-      </c>
+      <c r="L20" s="11"/>
       <c r="M20" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2714,16 +2730,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="12">
-        <v>7.9435400000000007E-3</v>
+        <v>-1.7651120000000001E-3</v>
       </c>
       <c r="C21" s="12">
-        <v>8.7541699999999997E-4</v>
+        <v>-1.372444733</v>
       </c>
       <c r="D21" s="12">
-        <v>-1.3629746279999999</v>
+        <v>-6.4936900000000001E-4</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>13</v>
@@ -2732,10 +2748,10 @@
         <v>3</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H21" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="14">
         <v>0.25</v>
@@ -2745,7 +2761,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L21" s="11"/>
+      <c r="L21" s="11">
+        <v>0</v>
+      </c>
       <c r="M21" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2753,16 +2771,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B22" s="12">
-        <v>-1.7651120000000001E-3</v>
+        <v>-2.9322559999999998E-3</v>
       </c>
       <c r="C22" s="12">
-        <v>-1.372444733</v>
+        <v>4.7167999999999998E-4</v>
       </c>
       <c r="D22" s="12">
-        <v>-6.4936900000000001E-4</v>
+        <v>1.3634863509999999</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>13</v>
@@ -2771,7 +2789,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H22" s="11">
         <v>1</v>
@@ -2784,9 +2802,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L22" s="11">
-        <v>0</v>
-      </c>
+      <c r="L22" s="11"/>
       <c r="M22" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2794,28 +2810,28 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="B23" s="12">
-        <v>-2.9322559999999998E-3</v>
+        <v>-8.6499899999999998E-4</v>
       </c>
       <c r="C23" s="12">
-        <v>4.7167999999999998E-4</v>
+        <v>1.3687832980000001</v>
       </c>
       <c r="D23" s="12">
-        <v>1.3634863509999999</v>
+        <v>-2.6270769999999998E-3</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H23" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="14">
         <v>0.25</v>
@@ -2825,7 +2841,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L23" s="11"/>
+      <c r="L23" s="11">
+        <v>0</v>
+      </c>
       <c r="M23" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2833,16 +2851,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B24" s="12">
-        <v>-8.6499899999999998E-4</v>
+        <v>-1.685024E-3</v>
       </c>
       <c r="C24" s="12">
-        <v>1.3687832980000001</v>
+        <v>1.9409000000000001E-4</v>
       </c>
       <c r="D24" s="12">
-        <v>-2.6270769999999998E-3</v>
+        <v>-1.362893881</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>13</v>
@@ -2851,7 +2869,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="11">
         <v>0</v>
@@ -2864,9 +2882,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L24" s="11">
-        <v>0</v>
-      </c>
+      <c r="L24" s="11"/>
       <c r="M24" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2874,16 +2890,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B25" s="12">
-        <v>-1.685024E-3</v>
+        <v>-3.7609869999999999E-3</v>
       </c>
       <c r="C25" s="12">
-        <v>1.9409000000000001E-4</v>
+        <v>-1.369220707</v>
       </c>
       <c r="D25" s="12">
-        <v>-1.362893881</v>
+        <v>2.3661670000000002E-3</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>13</v>
@@ -2892,10 +2908,10 @@
         <v>4</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H25" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="14">
         <v>0.25</v>
@@ -2905,7 +2921,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L25" s="11"/>
+      <c r="L25" s="11">
+        <v>0</v>
+      </c>
       <c r="M25" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -2913,16 +2931,16 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" s="12">
-        <v>-3.7609869999999999E-3</v>
+        <v>6.3251440000000004E-3</v>
       </c>
       <c r="C26" s="12">
-        <v>-1.369220707</v>
+        <v>3.1566400000000001E-4</v>
       </c>
       <c r="D26" s="12">
-        <v>2.3661670000000002E-3</v>
+        <v>1.363219121</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>13</v>
@@ -2931,7 +2949,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H26" s="11">
         <v>1</v>
@@ -2944,65 +2962,65 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L26" s="11">
-        <v>0</v>
-      </c>
+      <c r="L26" s="11"/>
       <c r="M26" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B27" s="12">
-        <v>6.3251440000000004E-3</v>
-      </c>
-      <c r="C27" s="12">
-        <v>3.1566400000000001E-4</v>
-      </c>
-      <c r="D27" s="12">
-        <v>1.363219121</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="13">
-        <v>4</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="11">
-        <v>1</v>
-      </c>
-      <c r="I27" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="14">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11">
+      <c r="A27" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="B27" s="15">
+        <v>-8.0833139999999994E-3</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1.369618539</v>
+      </c>
+      <c r="D27" s="15">
+        <v>3.1514800000000001E-4</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="17">
+        <v>5</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="18">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="L27" s="16">
+        <v>0</v>
+      </c>
+      <c r="M27" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B28" s="15">
-        <v>-8.0833139999999994E-3</v>
+        <v>7.2237580000000003E-3</v>
       </c>
       <c r="C28" s="15">
-        <v>1.369618539</v>
+        <v>-4.9644299999999995E-4</v>
       </c>
       <c r="D28" s="15">
-        <v>3.1514800000000001E-4</v>
+        <v>-1.362137393</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>14</v>
@@ -3011,7 +3029,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="16">
         <v>0</v>
@@ -3024,9 +3042,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L28" s="16">
-        <v>0</v>
-      </c>
+      <c r="L28" s="16"/>
       <c r="M28" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3034,16 +3050,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B29" s="15">
-        <v>7.2237580000000003E-3</v>
+        <v>-6.1688250000000002E-3</v>
       </c>
       <c r="C29" s="15">
-        <v>-4.9644299999999995E-4</v>
+        <v>-1.371633248</v>
       </c>
       <c r="D29" s="15">
-        <v>-1.362137393</v>
+        <v>-6.3095199999999999E-3</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>14</v>
@@ -3052,7 +3068,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H29" s="16">
         <v>0</v>
@@ -3065,7 +3081,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L29" s="16"/>
+      <c r="L29" s="16">
+        <v>0</v>
+      </c>
       <c r="M29" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3073,16 +3091,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B30" s="15">
-        <v>-6.1688250000000002E-3</v>
+        <v>6.8895800000000002E-3</v>
       </c>
       <c r="C30" s="15">
-        <v>-1.371633248</v>
+        <v>2.3354339999999999E-3</v>
       </c>
       <c r="D30" s="15">
-        <v>-6.3095199999999999E-3</v>
+        <v>1.3678903410000001</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>14</v>
@@ -3091,10 +3109,10 @@
         <v>5</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H30" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="18">
         <v>0.25</v>
@@ -3104,9 +3122,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
+      <c r="L30" s="16"/>
       <c r="M30" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3114,25 +3130,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>320</v>
+        <v>258</v>
       </c>
       <c r="B31" s="15">
-        <v>6.8895800000000002E-3</v>
+        <v>-4.404046E-3</v>
       </c>
       <c r="C31" s="15">
-        <v>2.3354339999999999E-3</v>
+        <v>1.3705249319999999</v>
       </c>
       <c r="D31" s="15">
-        <v>1.3678903410000001</v>
+        <v>6.7472000000000001E-3</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H31" s="16">
         <v>1</v>
@@ -3145,7 +3161,9 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L31" s="16"/>
+      <c r="L31" s="16">
+        <v>0</v>
+      </c>
       <c r="M31" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3153,16 +3171,16 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B32" s="15">
-        <v>-4.404046E-3</v>
+        <v>1.0746277E-2</v>
       </c>
       <c r="C32" s="15">
-        <v>1.3705249319999999</v>
+        <v>1.8556367000000001E-2</v>
       </c>
       <c r="D32" s="15">
-        <v>6.7472000000000001E-3</v>
+        <v>-1.364234722</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>14</v>
@@ -3171,10 +3189,10 @@
         <v>6</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="18">
         <v>0.25</v>
@@ -3184,9 +3202,7 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L32" s="16">
-        <v>0</v>
-      </c>
+      <c r="L32" s="16"/>
       <c r="M32" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3194,16 +3210,16 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B33" s="15">
-        <v>1.0746277E-2</v>
+        <v>-7.5468080000000003E-3</v>
       </c>
       <c r="C33" s="15">
-        <v>1.8556367000000001E-2</v>
+        <v>-1.3694108730000001</v>
       </c>
       <c r="D33" s="15">
-        <v>-1.364234722</v>
+        <v>-3.7574319999999998E-3</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>14</v>
@@ -3212,7 +3228,7 @@
         <v>6</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H33" s="16">
         <v>0</v>
@@ -3225,24 +3241,26 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L33" s="16"/>
+      <c r="L33" s="16">
+        <v>-4.9999999999999989E-2</v>
+      </c>
       <c r="M33" s="16">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B34" s="15">
-        <v>-7.5468080000000003E-3</v>
+        <v>1.040394E-3</v>
       </c>
       <c r="C34" s="15">
-        <v>-1.3694108730000001</v>
+        <v>-1.9971882E-2</v>
       </c>
       <c r="D34" s="15">
-        <v>-3.7574319999999998E-3</v>
+        <v>1.3615656439999999</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>14</v>
@@ -3251,61 +3269,61 @@
         <v>6</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H34" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="18">
         <v>0.25</v>
       </c>
       <c r="J34" s="16"/>
       <c r="K34" s="18">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="L34" s="16">
-        <v>-4.9999999999999989E-2</v>
-      </c>
+        <f t="shared" ref="K34:K65" si="2">I34+J34</f>
+        <v>0.25</v>
+      </c>
+      <c r="L34" s="16"/>
       <c r="M34" s="16">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="B35" s="15">
-        <v>1.040394E-3</v>
+        <v>3.7809200000000001E-3</v>
       </c>
       <c r="C35" s="15">
-        <v>-1.9971882E-2</v>
+        <v>1.370595107</v>
       </c>
       <c r="D35" s="15">
-        <v>1.3615656439999999</v>
+        <v>-8.2268570000000006E-3</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H35" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="18">
         <v>0.25</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="18">
-        <f t="shared" ref="K35:K66" si="2">I35+J35</f>
-        <v>0.25</v>
-      </c>
-      <c r="L35" s="16"/>
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0</v>
+      </c>
       <c r="M35" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3313,16 +3331,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B36" s="15">
-        <v>3.7809200000000001E-3</v>
+        <v>-2.2865149999999998E-3</v>
       </c>
       <c r="C36" s="15">
-        <v>1.370595107</v>
+        <v>-1.6584102E-2</v>
       </c>
       <c r="D36" s="15">
-        <v>-8.2268570000000006E-3</v>
+        <v>-1.363632819</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>14</v>
@@ -3331,7 +3349,7 @@
         <v>7</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H36" s="16">
         <v>0</v>
@@ -3344,9 +3362,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L36" s="16">
-        <v>0</v>
-      </c>
+      <c r="L36" s="16"/>
       <c r="M36" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3354,16 +3370,16 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B37" s="15">
-        <v>-2.2865149999999998E-3</v>
+        <v>6.8774719999999999E-3</v>
       </c>
       <c r="C37" s="15">
-        <v>-1.6584102E-2</v>
+        <v>-1.3733725000000001</v>
       </c>
       <c r="D37" s="15">
-        <v>-1.363632819</v>
+        <v>6.6301670000000002E-3</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>14</v>
@@ -3372,7 +3388,7 @@
         <v>7</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H37" s="16">
         <v>0</v>
@@ -3385,7 +3401,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L37" s="16"/>
+      <c r="L37" s="16">
+        <v>0</v>
+      </c>
       <c r="M37" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3393,16 +3411,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B38" s="15">
-        <v>6.8774719999999999E-3</v>
+        <v>-8.4238339999999998E-3</v>
       </c>
       <c r="C38" s="15">
-        <v>-1.3733725000000001</v>
+        <v>1.9623907999999999E-2</v>
       </c>
       <c r="D38" s="15">
-        <v>6.6301670000000002E-3</v>
+        <v>1.365223117</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>14</v>
@@ -3411,10 +3429,10 @@
         <v>7</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H38" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="18">
         <v>0.25</v>
@@ -3424,65 +3442,65 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L38" s="16">
-        <v>0</v>
-      </c>
+      <c r="L38" s="16"/>
       <c r="M38" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="B39" s="15">
-        <v>-8.4238339999999998E-3</v>
-      </c>
-      <c r="C39" s="15">
-        <v>1.9623907999999999E-2</v>
-      </c>
-      <c r="D39" s="15">
-        <v>1.365223117</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="17">
-        <v>7</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H39" s="16">
-        <v>1</v>
-      </c>
-      <c r="I39" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="J39" s="16"/>
-      <c r="K39" s="18">
+      <c r="A39" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B39" s="12">
+        <v>1.0954490000000001E-3</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1.368916603</v>
+      </c>
+      <c r="D39" s="12">
+        <v>3.5613910000000001E-3</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="13">
+        <v>8</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0</v>
+      </c>
+      <c r="I39" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="14">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16">
+      <c r="L39" s="11">
+        <v>0</v>
+      </c>
+      <c r="M39" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B40" s="12">
-        <v>1.0954490000000001E-3</v>
+        <v>-1.557061E-3</v>
       </c>
       <c r="C40" s="12">
-        <v>1.368916603</v>
+        <v>-1.7420715999999999E-2</v>
       </c>
       <c r="D40" s="12">
-        <v>3.5613910000000001E-3</v>
+        <v>-1.366031816</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>15</v>
@@ -3491,7 +3509,7 @@
         <v>8</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H40" s="11">
         <v>0</v>
@@ -3504,9 +3522,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L40" s="11">
-        <v>0</v>
-      </c>
+      <c r="L40" s="11"/>
       <c r="M40" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3514,16 +3530,16 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B41" s="12">
-        <v>-1.557061E-3</v>
+        <v>-7.6538109999999999E-3</v>
       </c>
       <c r="C41" s="12">
-        <v>-1.7420715999999999E-2</v>
+        <v>-1.3693474889999999</v>
       </c>
       <c r="D41" s="12">
-        <v>-1.366031816</v>
+        <v>-1.6735929999999999E-3</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>15</v>
@@ -3532,7 +3548,7 @@
         <v>8</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H41" s="11">
         <v>0</v>
@@ -3545,7 +3561,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L41" s="11"/>
+      <c r="L41" s="11">
+        <v>0</v>
+      </c>
       <c r="M41" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3553,16 +3571,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B42" s="12">
-        <v>-7.6538109999999999E-3</v>
+        <v>8.2259010000000007E-3</v>
       </c>
       <c r="C42" s="12">
-        <v>-1.3693474889999999</v>
+        <v>1.7832704000000001E-2</v>
       </c>
       <c r="D42" s="12">
-        <v>-1.6735929999999999E-3</v>
+        <v>1.364274794</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>15</v>
@@ -3571,10 +3589,10 @@
         <v>8</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H42" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="14">
         <v>0.25</v>
@@ -3584,9 +3602,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L42" s="11">
-        <v>0</v>
-      </c>
+      <c r="L42" s="11"/>
       <c r="M42" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3594,25 +3610,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="B43" s="12">
-        <v>8.2259010000000007E-3</v>
+        <v>-1.2860458999999999E-2</v>
       </c>
       <c r="C43" s="12">
-        <v>1.7832704000000001E-2</v>
+        <v>1.3691310750000001</v>
       </c>
       <c r="D43" s="12">
-        <v>1.364274794</v>
+        <v>-7.8760089999999998E-3</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H43" s="11">
         <v>1</v>
@@ -3625,7 +3641,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L43" s="11"/>
+      <c r="L43" s="11">
+        <v>0</v>
+      </c>
       <c r="M43" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3633,16 +3651,16 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B44" s="12">
-        <v>-1.2860458999999999E-2</v>
+        <v>1.2023123E-2</v>
       </c>
       <c r="C44" s="12">
-        <v>1.3691310750000001</v>
+        <v>-2.0042025000000002E-2</v>
       </c>
       <c r="D44" s="12">
-        <v>-7.8760089999999998E-3</v>
+        <v>-1.3632170020000001</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>15</v>
@@ -3651,10 +3669,10 @@
         <v>9</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H44" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="14">
         <v>0.25</v>
@@ -3664,9 +3682,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L44" s="11">
-        <v>0</v>
-      </c>
+      <c r="L44" s="11"/>
       <c r="M44" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3674,16 +3690,16 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B45" s="12">
-        <v>1.2023123E-2</v>
+        <v>7.7330680000000001E-3</v>
       </c>
       <c r="C45" s="12">
-        <v>-2.0042025000000002E-2</v>
+        <v>-1.3709505200000001</v>
       </c>
       <c r="D45" s="12">
-        <v>-1.3632170020000001</v>
+        <v>5.4873659999999996E-3</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>15</v>
@@ -3692,7 +3708,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H45" s="11">
         <v>0</v>
@@ -3705,7 +3721,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L45" s="11"/>
+      <c r="L45" s="11">
+        <v>0</v>
+      </c>
       <c r="M45" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3713,16 +3731,16 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B46" s="12">
-        <v>7.7330680000000001E-3</v>
+        <v>-6.427065E-3</v>
       </c>
       <c r="C46" s="12">
-        <v>-1.3709505200000001</v>
+        <v>2.1736674000000001E-2</v>
       </c>
       <c r="D46" s="12">
-        <v>5.4873659999999996E-3</v>
+        <v>1.3657281080000001</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>15</v>
@@ -3731,10 +3749,10 @@
         <v>9</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H46" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="14">
         <v>0.25</v>
@@ -3744,9 +3762,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L46" s="11">
-        <v>0</v>
-      </c>
+      <c r="L46" s="11"/>
       <c r="M46" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3754,25 +3770,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="B47" s="12">
-        <v>-6.427065E-3</v>
+        <v>2.6339050000000002E-3</v>
       </c>
       <c r="C47" s="12">
-        <v>2.1736674000000001E-2</v>
+        <v>1.3705563629999999</v>
       </c>
       <c r="D47" s="12">
-        <v>1.3657281080000001</v>
+        <v>-1.030111E-3</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H47" s="11">
         <v>1</v>
@@ -3785,7 +3801,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L47" s="11"/>
+      <c r="L47" s="11">
+        <v>0</v>
+      </c>
       <c r="M47" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3793,16 +3811,16 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B48" s="12">
-        <v>2.6339050000000002E-3</v>
+        <v>7.1482050000000004E-3</v>
       </c>
       <c r="C48" s="12">
-        <v>1.3705563629999999</v>
+        <v>-6.009927E-3</v>
       </c>
       <c r="D48" s="12">
-        <v>-1.030111E-3</v>
+        <v>-1.364986043</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>15</v>
@@ -3811,10 +3829,10 @@
         <v>10</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H48" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="14">
         <v>0.25</v>
@@ -3824,9 +3842,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L48" s="11">
-        <v>0</v>
-      </c>
+      <c r="L48" s="11"/>
       <c r="M48" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3834,16 +3850,16 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" s="12">
-        <v>7.1482050000000004E-3</v>
+        <v>3.822317E-3</v>
       </c>
       <c r="C49" s="12">
-        <v>-6.009927E-3</v>
+        <v>-1.371257918</v>
       </c>
       <c r="D49" s="12">
-        <v>-1.364986043</v>
+        <v>2.71653E-3</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>15</v>
@@ -3852,7 +3868,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H49" s="11">
         <v>0</v>
@@ -3865,7 +3881,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L49" s="11"/>
+      <c r="L49" s="11">
+        <v>0</v>
+      </c>
       <c r="M49" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3873,16 +3891,16 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B50" s="12">
-        <v>3.822317E-3</v>
+        <v>-1.3664624E-2</v>
       </c>
       <c r="C50" s="12">
-        <v>-1.371257918</v>
+        <v>6.706895E-3</v>
       </c>
       <c r="D50" s="12">
-        <v>2.71653E-3</v>
+        <v>1.363259837</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>15</v>
@@ -3891,10 +3909,10 @@
         <v>10</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="14">
         <v>0.25</v>
@@ -3904,65 +3922,65 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L50" s="11">
-        <v>0</v>
-      </c>
+      <c r="L50" s="11"/>
       <c r="M50" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" s="12">
-        <v>-1.3664624E-2</v>
-      </c>
-      <c r="C51" s="12">
-        <v>6.706895E-3</v>
-      </c>
-      <c r="D51" s="12">
-        <v>1.363259837</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="13">
-        <v>10</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H51" s="11">
-        <v>1</v>
-      </c>
-      <c r="I51" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="J51" s="11"/>
-      <c r="K51" s="14">
+      <c r="A51" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="15">
+        <v>1.7300830000000001E-3</v>
+      </c>
+      <c r="C51" s="15">
+        <v>1.3704968500000001</v>
+      </c>
+      <c r="D51" s="15">
+        <v>-1.363562E-3</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="17">
+        <v>11</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="16">
+        <v>1</v>
+      </c>
+      <c r="I51" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="J51" s="16"/>
+      <c r="K51" s="18">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11">
+      <c r="L51" s="16">
+        <v>0</v>
+      </c>
+      <c r="M51" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B52" s="15">
-        <v>1.7300830000000001E-3</v>
+        <v>-3.7967399999999998E-4</v>
       </c>
       <c r="C52" s="15">
-        <v>1.3704968500000001</v>
+        <v>-1.7741896E-2</v>
       </c>
       <c r="D52" s="15">
-        <v>-1.363562E-3</v>
+        <v>-1.362854096</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>16</v>
@@ -3971,10 +3989,10 @@
         <v>11</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H52" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="18">
         <v>0.25</v>
@@ -3984,9 +4002,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L52" s="16">
-        <v>0</v>
-      </c>
+      <c r="L52" s="16"/>
       <c r="M52" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -3994,16 +4010,16 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B53" s="15">
-        <v>-3.7967399999999998E-4</v>
+        <v>-2.1480700000000002E-3</v>
       </c>
       <c r="C53" s="15">
-        <v>-1.7741896E-2</v>
+        <v>-1.3719686</v>
       </c>
       <c r="D53" s="15">
-        <v>-1.362854096</v>
+        <v>-2.2418659999999999E-3</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>16</v>
@@ -4012,10 +4028,10 @@
         <v>11</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H53" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="18">
         <v>0.25</v>
@@ -4025,7 +4041,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L53" s="16"/>
+      <c r="L53" s="16">
+        <v>0</v>
+      </c>
       <c r="M53" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4033,16 +4051,16 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B54" s="15">
-        <v>-2.1480700000000002E-3</v>
+        <v>7.9338800000000001E-4</v>
       </c>
       <c r="C54" s="15">
-        <v>-1.3719686</v>
+        <v>1.9127938000000001E-2</v>
       </c>
       <c r="D54" s="15">
-        <v>-2.2418659999999999E-3</v>
+        <v>1.3664511100000001</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>16</v>
@@ -4051,7 +4069,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H54" s="16">
         <v>1</v>
@@ -4064,9 +4082,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L54" s="16">
-        <v>0</v>
-      </c>
+      <c r="L54" s="16"/>
       <c r="M54" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4074,28 +4090,28 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>104</v>
+        <v>262</v>
       </c>
       <c r="B55" s="15">
-        <v>7.9338800000000001E-4</v>
+        <v>-1.4783349999999999E-3</v>
       </c>
       <c r="C55" s="15">
-        <v>1.9127938000000001E-2</v>
+        <v>1.3689076790000001</v>
       </c>
       <c r="D55" s="15">
-        <v>1.3664511100000001</v>
+        <v>1.1494079000000001E-2</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F55" s="17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H55" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="18">
         <v>0.25</v>
@@ -4105,7 +4121,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L55" s="16"/>
+      <c r="L55" s="16">
+        <v>0</v>
+      </c>
       <c r="M55" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4113,16 +4131,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B56" s="15">
-        <v>-1.4783349999999999E-3</v>
+        <v>4.9091079999999997E-3</v>
       </c>
       <c r="C56" s="15">
-        <v>1.3689076790000001</v>
+        <v>-1.869053E-2</v>
       </c>
       <c r="D56" s="15">
-        <v>1.1494079000000001E-2</v>
+        <v>-1.3637116199999999</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>16</v>
@@ -4131,7 +4149,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H56" s="16">
         <v>0</v>
@@ -4144,9 +4162,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L56" s="16">
-        <v>0</v>
-      </c>
+      <c r="L56" s="16"/>
       <c r="M56" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4154,16 +4170,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B57" s="15">
-        <v>4.9091079999999997E-3</v>
+        <v>-1.0638989E-2</v>
       </c>
       <c r="C57" s="15">
-        <v>-1.869053E-2</v>
+        <v>-1.3712746899999999</v>
       </c>
       <c r="D57" s="15">
-        <v>-1.3637116199999999</v>
+        <v>-1.2683771E-2</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>16</v>
@@ -4172,10 +4188,10 @@
         <v>12</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H57" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="18">
         <v>0.25</v>
@@ -4185,7 +4201,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L57" s="16"/>
+      <c r="L57" s="16">
+        <v>0</v>
+      </c>
       <c r="M57" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4193,16 +4211,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B58" s="15">
-        <v>-1.0638989E-2</v>
+        <v>7.3743330000000003E-3</v>
       </c>
       <c r="C58" s="15">
-        <v>-1.3712746899999999</v>
+        <v>2.1104629E-2</v>
       </c>
       <c r="D58" s="15">
-        <v>-1.2683771E-2</v>
+        <v>1.364868747</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>16</v>
@@ -4211,7 +4229,7 @@
         <v>12</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H58" s="16">
         <v>1</v>
@@ -4224,9 +4242,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L58" s="16">
-        <v>0</v>
-      </c>
+      <c r="L58" s="16"/>
       <c r="M58" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4234,28 +4250,28 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>265</v>
+        <v>97</v>
       </c>
       <c r="B59" s="15">
-        <v>7.3743330000000003E-3</v>
+        <v>-1.858122E-3</v>
       </c>
       <c r="C59" s="15">
-        <v>2.1104629E-2</v>
+        <v>1.3706402070000001</v>
       </c>
       <c r="D59" s="15">
-        <v>1.364868747</v>
+        <v>-6.2848039999999997E-3</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H59" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="18">
         <v>0.25</v>
@@ -4265,7 +4281,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L59" s="16"/>
+      <c r="L59" s="16">
+        <v>0</v>
+      </c>
       <c r="M59" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4273,16 +4291,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B60" s="15">
-        <v>-1.858122E-3</v>
+        <v>4.6346740000000001E-3</v>
       </c>
       <c r="C60" s="15">
-        <v>1.3706402070000001</v>
+        <v>-1.3505634000000001E-2</v>
       </c>
       <c r="D60" s="15">
-        <v>-6.2848039999999997E-3</v>
+        <v>-1.3603634339999999</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>16</v>
@@ -4291,7 +4309,7 @@
         <v>13</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H60" s="16">
         <v>0</v>
@@ -4304,9 +4322,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L60" s="16">
-        <v>0</v>
-      </c>
+      <c r="L60" s="16"/>
       <c r="M60" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4314,16 +4330,16 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B61" s="15">
-        <v>4.6346740000000001E-3</v>
+        <v>-6.8489900000000001E-3</v>
       </c>
       <c r="C61" s="15">
-        <v>-1.3505634000000001E-2</v>
+        <v>-1.3701617420000001</v>
       </c>
       <c r="D61" s="15">
-        <v>-1.3603634339999999</v>
+        <v>3.37763E-3</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>16</v>
@@ -4332,10 +4348,10 @@
         <v>13</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H61" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="18">
         <v>0.25</v>
@@ -4345,7 +4361,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L61" s="16"/>
+      <c r="L61" s="16">
+        <v>0</v>
+      </c>
       <c r="M61" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4353,16 +4371,16 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B62" s="15">
-        <v>-6.8489900000000001E-3</v>
+        <v>4.097776E-3</v>
       </c>
       <c r="C62" s="15">
-        <v>-1.3701617420000001</v>
+        <v>1.3061092E-2</v>
       </c>
       <c r="D62" s="15">
-        <v>3.37763E-3</v>
+        <v>1.3631872009999999</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>16</v>
@@ -4371,7 +4389,7 @@
         <v>13</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H62" s="16">
         <v>1</v>
@@ -4384,65 +4402,65 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L62" s="16">
-        <v>0</v>
-      </c>
+      <c r="L62" s="16"/>
       <c r="M62" s="16">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="15">
-        <v>4.097776E-3</v>
-      </c>
-      <c r="C63" s="15">
-        <v>1.3061092E-2</v>
-      </c>
-      <c r="D63" s="15">
-        <v>1.3631872009999999</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="17">
-        <v>13</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H63" s="16">
-        <v>1</v>
-      </c>
-      <c r="I63" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="J63" s="16"/>
-      <c r="K63" s="18">
+      <c r="A63" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="12">
+        <v>-3.4898479999999998E-3</v>
+      </c>
+      <c r="C63" s="12">
+        <v>1.3715938780000001</v>
+      </c>
+      <c r="D63" s="12">
+        <v>-1.9695820000000001E-3</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="13">
+        <v>14</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="11">
+        <v>1</v>
+      </c>
+      <c r="I63" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J63" s="11"/>
+      <c r="K63" s="14">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L63" s="16"/>
-      <c r="M63" s="16">
+      <c r="L63" s="11">
+        <v>0</v>
+      </c>
+      <c r="M63" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B64" s="12">
-        <v>-3.4898479999999998E-3</v>
+        <v>1.1647823999999999E-2</v>
       </c>
       <c r="C64" s="12">
-        <v>1.3715938780000001</v>
+        <v>1.4750340000000001E-3</v>
       </c>
       <c r="D64" s="12">
-        <v>-1.9695820000000001E-3</v>
+        <v>-1.3623692810000001</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>17</v>
@@ -4451,10 +4469,10 @@
         <v>14</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H64" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="14">
         <v>0.25</v>
@@ -4464,9 +4482,7 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L64" s="11">
-        <v>0</v>
-      </c>
+      <c r="L64" s="11"/>
       <c r="M64" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4474,16 +4490,16 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B65" s="12">
-        <v>1.1647823999999999E-2</v>
+        <v>-7.9727359999999994E-3</v>
       </c>
       <c r="C65" s="12">
-        <v>1.4750340000000001E-3</v>
+        <v>-1.3701255189999999</v>
       </c>
       <c r="D65" s="12">
-        <v>-1.3623692810000001</v>
+        <v>-6.9298700000000005E-4</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>17</v>
@@ -4492,10 +4508,10 @@
         <v>14</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H65" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="14">
         <v>0.25</v>
@@ -4505,7 +4521,9 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L65" s="11"/>
+      <c r="L65" s="11">
+        <v>0</v>
+      </c>
       <c r="M65" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4513,16 +4531,16 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B66" s="12">
-        <v>-7.9727359999999994E-3</v>
+        <v>-9.1250599999999997E-5</v>
       </c>
       <c r="C66" s="12">
-        <v>-1.3701255189999999</v>
+        <v>-2.8483139999999998E-3</v>
       </c>
       <c r="D66" s="12">
-        <v>-6.9298700000000005E-4</v>
+        <v>1.3649904239999999</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>17</v>
@@ -4531,7 +4549,7 @@
         <v>14</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H66" s="11">
         <v>1</v>
@@ -4541,12 +4559,10 @@
       </c>
       <c r="J66" s="11"/>
       <c r="K66" s="14">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="L66" s="11">
-        <v>0</v>
-      </c>
+        <f t="shared" ref="K66:K97" si="3">I66+J66</f>
+        <v>0.25</v>
+      </c>
+      <c r="L66" s="11"/>
       <c r="M66" s="11">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -4554,55 +4570,57 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="B67" s="12">
-        <v>-9.1250599999999997E-5</v>
+        <v>8.9010499999999998E-4</v>
       </c>
       <c r="C67" s="12">
-        <v>-2.8483139999999998E-3</v>
+        <v>1.3706640269999999</v>
       </c>
       <c r="D67" s="12">
-        <v>1.3649904239999999</v>
+        <v>-4.5450680000000002E-3</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F67" s="13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H67" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="14">
         <v>0.25</v>
       </c>
       <c r="J67" s="11"/>
       <c r="K67" s="14">
-        <f t="shared" ref="K67:K98" si="3">I67+J67</f>
-        <v>0.25</v>
-      </c>
-      <c r="L67" s="11"/>
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="L67" s="11">
+        <v>0</v>
+      </c>
       <c r="M67" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M67:M102" si="4">L67+K67</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B68" s="12">
-        <v>8.9010499999999998E-4</v>
+        <v>-3.4156849999999999E-3</v>
       </c>
       <c r="C68" s="12">
-        <v>1.3706640269999999</v>
+        <v>1.7018775999999999E-2</v>
       </c>
       <c r="D68" s="12">
-        <v>-4.5450680000000002E-3</v>
+        <v>-1.3617754399999999</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>17</v>
@@ -4611,7 +4629,7 @@
         <v>15</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H68" s="11">
         <v>0</v>
@@ -4624,26 +4642,24 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L68" s="11">
-        <v>0</v>
-      </c>
+      <c r="L68" s="11"/>
       <c r="M68" s="11">
-        <f t="shared" ref="M68:M103" si="4">L68+K68</f>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B69" s="12">
-        <v>-3.4156849999999999E-3</v>
+        <v>-4.6379630000000002E-3</v>
       </c>
       <c r="C69" s="12">
-        <v>1.7018775999999999E-2</v>
+        <v>-1.3699409339999999</v>
       </c>
       <c r="D69" s="12">
-        <v>-1.3617754399999999</v>
+        <v>2.0726799999999999E-3</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>17</v>
@@ -4652,7 +4668,7 @@
         <v>15</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H69" s="11">
         <v>0</v>
@@ -4665,7 +4681,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L69" s="11"/>
+      <c r="L69" s="11">
+        <v>0</v>
+      </c>
       <c r="M69" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4673,16 +4691,16 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B70" s="12">
-        <v>-4.6379630000000002E-3</v>
+        <v>7.2554330000000004E-3</v>
       </c>
       <c r="C70" s="12">
-        <v>-1.3699409339999999</v>
+        <v>-1.7726433E-2</v>
       </c>
       <c r="D70" s="12">
-        <v>2.0726799999999999E-3</v>
+        <v>1.364100275</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>17</v>
@@ -4691,10 +4709,10 @@
         <v>15</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H70" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="14">
         <v>0.25</v>
@@ -4704,9 +4722,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L70" s="11">
-        <v>0</v>
-      </c>
+      <c r="L70" s="11"/>
       <c r="M70" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4714,28 +4730,28 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
       <c r="B71" s="12">
-        <v>7.2554330000000004E-3</v>
+        <v>1.3188531999999999E-2</v>
       </c>
       <c r="C71" s="12">
-        <v>-1.7726433E-2</v>
+        <v>1.370234613</v>
       </c>
       <c r="D71" s="12">
-        <v>1.364100275</v>
+        <v>-1.805393E-3</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F71" s="13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H71" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="14">
         <v>0.25</v>
@@ -4745,7 +4761,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L71" s="11"/>
+      <c r="L71" s="11">
+        <v>0</v>
+      </c>
       <c r="M71" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4753,16 +4771,16 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B72" s="12">
-        <v>1.3188531999999999E-2</v>
+        <v>-1.0831491E-2</v>
       </c>
       <c r="C72" s="12">
-        <v>1.370234613</v>
+        <v>2.1504664E-2</v>
       </c>
       <c r="D72" s="12">
-        <v>-1.805393E-3</v>
+        <v>-1.3637596809999999</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>17</v>
@@ -4771,7 +4789,7 @@
         <v>16</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H72" s="11">
         <v>0</v>
@@ -4784,9 +4802,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L72" s="11">
-        <v>0</v>
-      </c>
+      <c r="L72" s="11"/>
       <c r="M72" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4794,16 +4810,16 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B73" s="12">
-        <v>-1.0831491E-2</v>
+        <v>-1.0091199E-2</v>
       </c>
       <c r="C73" s="12">
-        <v>2.1504664E-2</v>
+        <v>-1.3700456489999999</v>
       </c>
       <c r="D73" s="12">
-        <v>-1.3637596809999999</v>
+        <v>1.9584479999999998E-3</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>17</v>
@@ -4812,7 +4828,7 @@
         <v>16</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H73" s="11">
         <v>0</v>
@@ -4825,7 +4841,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L73" s="11"/>
+      <c r="L73" s="11">
+        <v>0</v>
+      </c>
       <c r="M73" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4833,16 +4851,16 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B74" s="12">
-        <v>-1.0091199E-2</v>
+        <v>7.5917989999999998E-3</v>
       </c>
       <c r="C74" s="12">
-        <v>-1.3700456489999999</v>
+        <v>-2.1907407E-2</v>
       </c>
       <c r="D74" s="12">
-        <v>1.9584479999999998E-3</v>
+        <v>1.363887176</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>17</v>
@@ -4851,10 +4869,10 @@
         <v>16</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H74" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" s="14">
         <v>0.25</v>
@@ -4864,65 +4882,65 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L74" s="11">
-        <v>0</v>
-      </c>
+      <c r="L74" s="11"/>
       <c r="M74" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="B75" s="12">
-        <v>7.5917989999999998E-3</v>
-      </c>
-      <c r="C75" s="12">
-        <v>-2.1907407E-2</v>
-      </c>
-      <c r="D75" s="12">
-        <v>1.363887176</v>
-      </c>
-      <c r="E75" s="11" t="s">
+      <c r="A75" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="15">
+        <v>-2.031E-5</v>
+      </c>
+      <c r="C75" s="15">
+        <v>1.369789691</v>
+      </c>
+      <c r="D75" s="15">
+        <v>-7.1691580000000001E-3</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="17">
         <v>17</v>
       </c>
-      <c r="F75" s="13">
-        <v>16</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H75" s="11">
-        <v>1</v>
-      </c>
-      <c r="I75" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="J75" s="11"/>
-      <c r="K75" s="14">
+      <c r="G75" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" s="16">
+        <v>0</v>
+      </c>
+      <c r="I75" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="J75" s="16"/>
+      <c r="K75" s="18">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L75" s="11"/>
-      <c r="M75" s="11">
+      <c r="L75" s="16">
+        <v>0</v>
+      </c>
+      <c r="M75" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B76" s="15">
-        <v>-2.031E-5</v>
+        <v>-6.6080460000000002E-3</v>
       </c>
       <c r="C76" s="15">
-        <v>1.369789691</v>
+        <v>5.4102109999999998E-3</v>
       </c>
       <c r="D76" s="15">
-        <v>-7.1691580000000001E-3</v>
+        <v>-1.3643928249999999</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>18</v>
@@ -4931,7 +4949,7 @@
         <v>17</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H76" s="16">
         <v>0</v>
@@ -4944,9 +4962,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L76" s="16">
-        <v>0</v>
-      </c>
+      <c r="L76" s="16"/>
       <c r="M76" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4954,16 +4970,16 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B77" s="15">
-        <v>-6.6080460000000002E-3</v>
+        <v>9.9050809999999996E-3</v>
       </c>
       <c r="C77" s="15">
-        <v>5.4102109999999998E-3</v>
+        <v>-1.371059048</v>
       </c>
       <c r="D77" s="15">
-        <v>-1.3643928249999999</v>
+        <v>8.5651579999999998E-3</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>18</v>
@@ -4972,10 +4988,10 @@
         <v>17</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H77" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" s="18">
         <v>0.25</v>
@@ -4985,7 +5001,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L77" s="16"/>
+      <c r="L77" s="16">
+        <v>0</v>
+      </c>
       <c r="M77" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -4993,16 +5011,16 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B78" s="15">
-        <v>9.9050809999999996E-3</v>
+        <v>-3.292456E-3</v>
       </c>
       <c r="C78" s="15">
-        <v>-1.371059048</v>
+        <v>-4.2145630000000002E-3</v>
       </c>
       <c r="D78" s="15">
-        <v>8.5651579999999998E-3</v>
+        <v>1.3628787389999999</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>18</v>
@@ -5011,7 +5029,7 @@
         <v>17</v>
       </c>
       <c r="G78" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H78" s="16">
         <v>1</v>
@@ -5024,9 +5042,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L78" s="16">
-        <v>0</v>
-      </c>
+      <c r="L78" s="16"/>
       <c r="M78" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5034,28 +5050,28 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="B79" s="15">
-        <v>-3.292456E-3</v>
+        <v>1.062271E-3</v>
       </c>
       <c r="C79" s="15">
-        <v>-4.2145630000000002E-3</v>
+        <v>1.37147372</v>
       </c>
       <c r="D79" s="15">
-        <v>1.3628787389999999</v>
+        <v>4.9500660000000004E-3</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F79" s="17">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H79" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="18">
         <v>0.25</v>
@@ -5065,7 +5081,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L79" s="16"/>
+      <c r="L79" s="16">
+        <v>0</v>
+      </c>
       <c r="M79" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5073,16 +5091,16 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B80" s="15">
-        <v>1.062271E-3</v>
+        <v>-3.392337E-3</v>
       </c>
       <c r="C80" s="15">
-        <v>1.37147372</v>
+        <v>-2.1573142999999999E-2</v>
       </c>
       <c r="D80" s="15">
-        <v>4.9500660000000004E-3</v>
+        <v>-1.365078131</v>
       </c>
       <c r="E80" s="16" t="s">
         <v>18</v>
@@ -5091,7 +5109,7 @@
         <v>18</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H80" s="16">
         <v>0</v>
@@ -5104,9 +5122,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L80" s="16">
-        <v>0</v>
-      </c>
+      <c r="L80" s="16"/>
       <c r="M80" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5114,16 +5130,16 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B81" s="15">
-        <v>-3.392337E-3</v>
+        <v>3.6929150000000002E-3</v>
       </c>
       <c r="C81" s="15">
-        <v>-2.1573142999999999E-2</v>
+        <v>-1.3699758040000001</v>
       </c>
       <c r="D81" s="15">
-        <v>-1.365078131</v>
+        <v>-3.3345169999999999E-3</v>
       </c>
       <c r="E81" s="16" t="s">
         <v>18</v>
@@ -5132,10 +5148,10 @@
         <v>18</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H81" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" s="18">
         <v>0.25</v>
@@ -5145,7 +5161,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L81" s="16"/>
+      <c r="L81" s="16">
+        <v>0</v>
+      </c>
       <c r="M81" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5153,16 +5171,16 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B82" s="15">
-        <v>3.6929150000000002E-3</v>
+        <v>-1.3792469999999999E-3</v>
       </c>
       <c r="C82" s="15">
-        <v>-1.3699758040000001</v>
+        <v>2.0191107999999999E-2</v>
       </c>
       <c r="D82" s="15">
-        <v>-3.3345169999999999E-3</v>
+        <v>1.3633974019999999</v>
       </c>
       <c r="E82" s="16" t="s">
         <v>18</v>
@@ -5171,7 +5189,7 @@
         <v>18</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H82" s="16">
         <v>1</v>
@@ -5184,9 +5202,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L82" s="16">
-        <v>0</v>
-      </c>
+      <c r="L82" s="16"/>
       <c r="M82" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5194,28 +5210,28 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B83" s="15">
-        <v>-1.3792469999999999E-3</v>
+        <v>-1.683925E-3</v>
       </c>
       <c r="C83" s="15">
-        <v>2.0191107999999999E-2</v>
+        <v>1.371166965</v>
       </c>
       <c r="D83" s="15">
-        <v>1.3633974019999999</v>
+        <v>1.0131459999999999E-3</v>
       </c>
       <c r="E83" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F83" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H83" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" s="18">
         <v>0.25</v>
@@ -5225,7 +5241,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L83" s="16"/>
+      <c r="L83" s="16">
+        <v>0</v>
+      </c>
       <c r="M83" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5233,16 +5251,16 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B84" s="15">
-        <v>-1.683925E-3</v>
+        <v>3.5831830000000002E-3</v>
       </c>
       <c r="C84" s="15">
-        <v>1.371166965</v>
+        <v>-1.5150614999999999E-2</v>
       </c>
       <c r="D84" s="15">
-        <v>1.0131459999999999E-3</v>
+        <v>-1.3617531839999999</v>
       </c>
       <c r="E84" s="16" t="s">
         <v>18</v>
@@ -5251,7 +5269,7 @@
         <v>19</v>
       </c>
       <c r="G84" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H84" s="16">
         <v>0</v>
@@ -5264,9 +5282,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L84" s="16">
-        <v>0</v>
-      </c>
+      <c r="L84" s="16"/>
       <c r="M84" s="16">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5274,16 +5290,16 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B85" s="15">
-        <v>3.5831830000000002E-3</v>
+        <v>-1.1879828E-2</v>
       </c>
       <c r="C85" s="15">
-        <v>-1.5150614999999999E-2</v>
+        <v>-1.3696255959999999</v>
       </c>
       <c r="D85" s="15">
-        <v>-1.3617531839999999</v>
+        <v>-6.8204549999999996E-3</v>
       </c>
       <c r="E85" s="16" t="s">
         <v>18</v>
@@ -5292,7 +5308,7 @@
         <v>19</v>
       </c>
       <c r="G85" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H85" s="16">
         <v>0</v>
@@ -5305,24 +5321,26 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L85" s="16"/>
+      <c r="L85" s="16">
+        <v>-4.9999999999999989E-2</v>
+      </c>
       <c r="M85" s="16">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B86" s="15">
-        <v>-1.1879828E-2</v>
+        <v>9.9863069999999998E-3</v>
       </c>
       <c r="C86" s="15">
-        <v>-1.3696255959999999</v>
+        <v>1.3495689E-2</v>
       </c>
       <c r="D86" s="15">
-        <v>-6.8204549999999996E-3</v>
+        <v>1.3675640019999999</v>
       </c>
       <c r="E86" s="16" t="s">
         <v>18</v>
@@ -5331,10 +5349,10 @@
         <v>19</v>
       </c>
       <c r="G86" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H86" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" s="18">
         <v>0.25</v>
@@ -5344,74 +5362,74 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L86" s="16">
-        <v>-4.9999999999999989E-2</v>
-      </c>
+      <c r="L86" s="16"/>
       <c r="M86" s="16">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B87" s="15">
-        <v>9.9863069999999998E-3</v>
-      </c>
-      <c r="C87" s="15">
-        <v>1.3495689E-2</v>
-      </c>
-      <c r="D87" s="15">
-        <v>1.3675640019999999</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F87" s="17">
-        <v>19</v>
-      </c>
-      <c r="G87" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H87" s="16">
-        <v>1</v>
-      </c>
-      <c r="I87" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="J87" s="16"/>
-      <c r="K87" s="18">
+      <c r="A87" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B87" s="12">
+        <v>1.801619E-3</v>
+      </c>
+      <c r="C87" s="12">
+        <v>1.3699387599999999</v>
+      </c>
+      <c r="D87" s="12">
+        <v>5.0315199999999998E-4</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="F87" s="13">
+        <v>20</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H87" s="11">
+        <v>0</v>
+      </c>
+      <c r="I87" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J87" s="11"/>
+      <c r="K87" s="14">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L87" s="16"/>
-      <c r="M87" s="16">
+      <c r="L87" s="11">
+        <v>0</v>
+      </c>
+      <c r="M87" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B88" s="12">
-        <v>1.801619E-3</v>
+        <v>-5.5391770000000002E-3</v>
       </c>
       <c r="C88" s="12">
-        <v>1.3699387599999999</v>
+        <v>1.5540164E-2</v>
       </c>
       <c r="D88" s="12">
-        <v>5.0315199999999998E-4</v>
+        <v>-1.360562284</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>451</v>
+        <v>19</v>
       </c>
       <c r="F88" s="13">
         <v>20</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H88" s="11">
         <v>0</v>
@@ -5424,9 +5442,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L88" s="11">
-        <v>0</v>
-      </c>
+      <c r="L88" s="11"/>
       <c r="M88" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5434,16 +5450,16 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B89" s="12">
-        <v>-5.5391770000000002E-3</v>
+        <v>-1.678981E-3</v>
       </c>
       <c r="C89" s="12">
-        <v>1.5540164E-2</v>
+        <v>-1.3703150690000001</v>
       </c>
       <c r="D89" s="12">
-        <v>-1.360562284</v>
+        <v>-3.612007E-3</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>19</v>
@@ -5452,10 +5468,10 @@
         <v>20</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H89" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" s="14">
         <v>0.25</v>
@@ -5465,7 +5481,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L89" s="11"/>
+      <c r="L89" s="11">
+        <v>0</v>
+      </c>
       <c r="M89" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5473,16 +5491,16 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B90" s="12">
-        <v>-1.678981E-3</v>
+        <v>5.4848739999999998E-3</v>
       </c>
       <c r="C90" s="12">
-        <v>-1.3703150690000001</v>
+        <v>-1.5202024999999999E-2</v>
       </c>
       <c r="D90" s="12">
-        <v>-3.612007E-3</v>
+        <v>1.363622396</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>19</v>
@@ -5491,7 +5509,7 @@
         <v>20</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H90" s="11">
         <v>1</v>
@@ -5504,9 +5522,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L90" s="11">
-        <v>0</v>
-      </c>
+      <c r="L90" s="11"/>
       <c r="M90" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5514,25 +5530,25 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="B91" s="12">
-        <v>5.4848739999999998E-3</v>
+        <v>1.433017E-3</v>
       </c>
       <c r="C91" s="12">
-        <v>-1.5202024999999999E-2</v>
+        <v>1.3693378970000001</v>
       </c>
       <c r="D91" s="12">
-        <v>1.363622396</v>
+        <v>3.2276100000000001E-3</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F91" s="13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H91" s="11">
         <v>1</v>
@@ -5545,7 +5561,9 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L91" s="11"/>
+      <c r="L91" s="11">
+        <v>0</v>
+      </c>
       <c r="M91" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5553,16 +5571,16 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B92" s="12">
-        <v>1.433017E-3</v>
+        <v>5.2994180000000002E-3</v>
       </c>
       <c r="C92" s="12">
-        <v>1.3693378970000001</v>
+        <v>1.5994611999999998E-2</v>
       </c>
       <c r="D92" s="12">
-        <v>3.2276100000000001E-3</v>
+        <v>-1.361729977</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>19</v>
@@ -5571,10 +5589,10 @@
         <v>21</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H92" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" s="14">
         <v>0.25</v>
@@ -5584,9 +5602,7 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L92" s="11">
-        <v>0</v>
-      </c>
+      <c r="L92" s="11"/>
       <c r="M92" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
@@ -5594,16 +5610,16 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B93" s="12">
-        <v>5.2994180000000002E-3</v>
+        <v>-1.2263557E-2</v>
       </c>
       <c r="C93" s="12">
-        <v>1.5994611999999998E-2</v>
+        <v>-1.3677908050000001</v>
       </c>
       <c r="D93" s="12">
-        <v>-1.361729977</v>
+        <v>-4.4754720000000003E-3</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>19</v>
@@ -5612,7 +5628,7 @@
         <v>21</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H93" s="11">
         <v>0</v>
@@ -5625,143 +5641,143 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L93" s="11"/>
+      <c r="L93" s="11">
+        <v>0</v>
+      </c>
       <c r="M93" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B94" s="12">
-        <v>-1.2263557E-2</v>
-      </c>
-      <c r="C94" s="12">
-        <v>-1.3677908050000001</v>
-      </c>
-      <c r="D94" s="12">
-        <v>-4.4754720000000003E-3</v>
-      </c>
-      <c r="E94" s="11" t="s">
+    <row r="94" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B94" s="25">
+        <v>5.5781270000000004E-3</v>
+      </c>
+      <c r="C94" s="25">
+        <v>-1.761735E-2</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1.363133943</v>
+      </c>
+      <c r="E94" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F94" s="13">
+      <c r="F94" s="26">
         <v>21</v>
       </c>
-      <c r="G94" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H94" s="11">
-        <v>0</v>
-      </c>
-      <c r="I94" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="J94" s="11"/>
-      <c r="K94" s="14">
+      <c r="G94" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H94" s="24">
+        <v>1</v>
+      </c>
+      <c r="I94" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="J94" s="24"/>
+      <c r="K94" s="27">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L94" s="11">
-        <v>0</v>
-      </c>
-      <c r="M94" s="11">
+      <c r="L94" s="24"/>
+      <c r="M94" s="24">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="B95" s="25">
-        <v>5.5781270000000004E-3</v>
-      </c>
-      <c r="C95" s="25">
-        <v>-1.761735E-2</v>
-      </c>
-      <c r="D95" s="25">
-        <v>1.363133943</v>
-      </c>
-      <c r="E95" s="24" t="s">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B95" s="9">
+        <v>3.6527180000000001E-3</v>
+      </c>
+      <c r="C95" s="9">
+        <v>1.3722747390000001</v>
+      </c>
+      <c r="D95" s="9">
+        <v>-7.55019E-4</v>
+      </c>
+      <c r="E95" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F95" s="26">
-        <v>21</v>
-      </c>
-      <c r="G95" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H95" s="24">
-        <v>1</v>
-      </c>
-      <c r="I95" s="27">
-        <v>0.25</v>
-      </c>
-      <c r="J95" s="24"/>
-      <c r="K95" s="27">
+      <c r="F95" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H95" s="8">
+        <v>0</v>
+      </c>
+      <c r="I95" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J95" s="8"/>
+      <c r="K95" s="3">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L95" s="24"/>
-      <c r="M95" s="24">
+      <c r="L95" s="8"/>
+      <c r="M95" s="8">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="B96" s="9">
-        <v>3.6527180000000001E-3</v>
-      </c>
-      <c r="C96" s="9">
-        <v>1.3722747390000001</v>
-      </c>
-      <c r="D96" s="9">
-        <v>-7.55019E-4</v>
-      </c>
-      <c r="E96" s="8" t="s">
+      <c r="A96" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="B96" s="12">
+        <v>1.3570100000000001E-3</v>
+      </c>
+      <c r="C96" s="12">
+        <v>1.3725135719999999</v>
+      </c>
+      <c r="D96" s="12">
+        <v>-5.5048349999999996E-3</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="F96" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="G96" s="8" t="s">
+      <c r="G96" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H96" s="8">
-        <v>0</v>
-      </c>
-      <c r="I96" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="J96" s="8"/>
-      <c r="K96" s="3">
+      <c r="H96" s="11">
+        <v>1</v>
+      </c>
+      <c r="I96" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J96" s="11"/>
+      <c r="K96" s="14">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8">
+      <c r="L96" s="11"/>
+      <c r="M96" s="11">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B97" s="12">
-        <v>1.3570100000000001E-3</v>
+        <v>-1.8163579999999999E-2</v>
       </c>
       <c r="C97" s="12">
-        <v>1.3725135719999999</v>
+        <v>1.3730120640000001</v>
       </c>
       <c r="D97" s="12">
-        <v>-5.5048349999999996E-3</v>
+        <v>3.4420689999999999E-3</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>19</v>
@@ -5773,7 +5789,7 @@
         <v>37</v>
       </c>
       <c r="H97" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" s="14">
         <v>0.25</v>
@@ -5791,16 +5807,16 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B98" s="12">
-        <v>-1.8163579999999999E-2</v>
+        <v>-4.410962E-3</v>
       </c>
       <c r="C98" s="12">
-        <v>1.3730120640000001</v>
+        <v>-6.1372110000000001E-3</v>
       </c>
       <c r="D98" s="12">
-        <v>3.4420689999999999E-3</v>
+        <v>-1.35304603</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>19</v>
@@ -5809,7 +5825,7 @@
         <v>373</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H98" s="11">
         <v>0</v>
@@ -5819,7 +5835,7 @@
       </c>
       <c r="J98" s="11"/>
       <c r="K98" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="K98:K102" si="5">I98+J98</f>
         <v>0.25</v>
       </c>
       <c r="L98" s="11"/>
@@ -5830,16 +5846,16 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B99" s="12">
-        <v>-4.410962E-3</v>
+        <v>5.079648E-3</v>
       </c>
       <c r="C99" s="12">
-        <v>-6.1372110000000001E-3</v>
+        <v>-9.5914750000000003E-3</v>
       </c>
       <c r="D99" s="12">
-        <v>-1.35304603</v>
+        <v>-1.354328183</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>19</v>
@@ -5858,7 +5874,7 @@
       </c>
       <c r="J99" s="11"/>
       <c r="K99" s="14">
-        <f t="shared" ref="K99:K130" si="5">I99+J99</f>
+        <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
       <c r="L99" s="11"/>
@@ -5869,16 +5885,16 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="B100" s="12">
-        <v>5.079648E-3</v>
+        <v>4.616546E-3</v>
       </c>
       <c r="C100" s="12">
-        <v>-9.5914750000000003E-3</v>
+        <v>-1.8255878999999999E-2</v>
       </c>
       <c r="D100" s="12">
-        <v>-1.354328183</v>
+        <v>-1.352590658</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>19</v>
@@ -5908,16 +5924,16 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="B101" s="12">
-        <v>4.616546E-3</v>
+        <v>-4.8617110000000003E-3</v>
       </c>
       <c r="C101" s="12">
-        <v>-1.8255878999999999E-2</v>
+        <v>-1.3740197329999999</v>
       </c>
       <c r="D101" s="12">
-        <v>-1.352590658</v>
+        <v>-3.78997E-4</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>19</v>
@@ -5926,10 +5942,10 @@
         <v>373</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H101" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" s="14">
         <v>0.25</v>
@@ -5947,16 +5963,16 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B102" s="12">
-        <v>-4.8617110000000003E-3</v>
+        <v>-8.7007330000000004E-3</v>
       </c>
       <c r="C102" s="12">
-        <v>-1.3740197329999999</v>
+        <v>-1.6625870000000001E-2</v>
       </c>
       <c r="D102" s="12">
-        <v>-3.78997E-4</v>
+        <v>1.353411567</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>19</v>
@@ -5965,7 +5981,7 @@
         <v>373</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H102" s="11">
         <v>1</v>
@@ -5984,49 +6000,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="B103" s="12">
-        <v>-8.7007330000000004E-3</v>
-      </c>
-      <c r="C103" s="12">
-        <v>-1.6625870000000001E-2</v>
-      </c>
-      <c r="D103" s="12">
-        <v>1.353411567</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="G103" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H103" s="11">
-        <v>1</v>
-      </c>
-      <c r="I103" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="J103" s="11"/>
-      <c r="K103" s="14">
-        <f t="shared" si="5"/>
-        <v>0.25</v>
-      </c>
-      <c r="L103" s="11"/>
-      <c r="M103" s="11">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
-  </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="598" r:id="rId1"/>
 </worksheet>

</xml_diff>